<commit_message>
Upload Documentation PDF for Runtime measurements and Analysis
Note: I am complier with old requirements as I
 have delivered old task requirement before.
- I just have an issue that's why project still open.
- I have resolved the issue and Task scheduling is working properly now.
</commit_message>
<xml_diff>
--- a/Doc/EDF Analysis.xlsx
+++ b/Doc/EDF Analysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MF\Personal\Intellectual\Embedded_SW\EgFWD\Advanced Embedded Systems\Course Material\RTOS\RTOS_SourceFiles\FreeRTOSv202112.00\FreeRTOS\Demo\RTOS_EDF_Scheduler_Project\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93294388-F299-48F3-AFC6-5A7EB062EB83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494ECEA2-7446-4669-9B6D-C4347851974E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6CDFFFD7-E2CF-4A8B-A352-0E908AB31361}"/>
   </bookViews>
@@ -34,9 +34,84 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
+  <si>
+    <t>Task 1</t>
+  </si>
+  <si>
+    <t>Task 2</t>
+  </si>
+  <si>
+    <t>Task 3</t>
+  </si>
+  <si>
+    <t>Task 4</t>
+  </si>
+  <si>
+    <t>Task name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task Periodicity(ms) </t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>20ms</t>
+  </si>
+  <si>
+    <t>40ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50ms </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10ms </t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>Hyper Period</t>
+  </si>
+  <si>
+    <t>Max (us)</t>
+  </si>
+  <si>
+    <t>Execution Time (us)</t>
+  </si>
+  <si>
+    <t>Task Name</t>
+  </si>
+  <si>
+    <t>Peridicity (ms)</t>
+  </si>
+  <si>
+    <t>Expected worst case
+Execution Time (usec)</t>
+  </si>
+  <si>
+    <t>Task execution Time during Hyper Period (200ms)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Execution During Hyper Period </t>
+  </si>
+  <si>
+    <t>CPU load %</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,16 +119,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3300"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -62,22 +182,96 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -85,6 +279,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF3300"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -393,59 +592,462 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27472322-B058-43E0-B473-93A72FD3F7DD}">
-  <dimension ref="D10:V11"/>
+  <dimension ref="A3:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="10" spans="4:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="4:22" x14ac:dyDescent="0.35">
-      <c r="D11" s="1">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1">
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1">
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="B6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
+        <v>0</v>
+      </c>
+      <c r="B7" s="5">
+        <v>13.3</v>
+      </c>
+      <c r="C7" s="6">
+        <v>24.6</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="8">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="26" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
+        <v>10</v>
+      </c>
+      <c r="B8" s="5">
+        <v>13.5</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="I8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
+        <v>20</v>
+      </c>
+      <c r="B9" s="5">
+        <v>13.5</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="7">
+        <v>25.15</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="I9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4">
+        <v>10</v>
+      </c>
+      <c r="K9" s="4">
+        <f>MAX(B7:B27)</f>
+        <v>14</v>
+      </c>
+      <c r="L9" s="4">
+        <f>(200/J9)*K9*(1/1000)</f>
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
         <v>30</v>
       </c>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1">
+      <c r="B10" s="5">
+        <v>13.35</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="I10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="4">
+        <v>50</v>
+      </c>
+      <c r="K10" s="4">
+        <f>MAX(C7:C27)</f>
+        <v>24.9</v>
+      </c>
+      <c r="L10" s="4">
+        <f t="shared" ref="L10:L12" si="0">(200/J10)*K10*(1/1000)</f>
+        <v>9.9599999999999994E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
+        <f>A10+10</f>
         <v>40</v>
       </c>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1">
+      <c r="B11" s="5">
+        <v>13.9</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="7">
+        <v>25</v>
+      </c>
+      <c r="E11" s="8">
+        <v>15.78</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="4">
+        <v>20</v>
+      </c>
+      <c r="K11" s="4">
+        <f>MAX(D7:D27)</f>
+        <v>25.2</v>
+      </c>
+      <c r="L11" s="4">
+        <f t="shared" si="0"/>
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
+        <f t="shared" ref="A12:A27" si="1">A11+10</f>
         <v>50</v>
       </c>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1">
+      <c r="B12" s="5">
+        <v>13.38</v>
+      </c>
+      <c r="C12" s="6">
+        <v>24.9</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="I12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" s="4">
+        <v>40</v>
+      </c>
+      <c r="K12" s="4">
+        <f>MAX(E7:E27)</f>
+        <v>15.78</v>
+      </c>
+      <c r="L12" s="4">
+        <f t="shared" si="0"/>
+        <v>7.8899999999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1">
+      <c r="B13" s="5">
+        <v>13.4</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="7">
+        <v>25.2</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="I13" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="4">
+        <f>SUM(L9:L12)</f>
+        <v>0.71050000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="4">
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1">
+      <c r="B14" s="5">
+        <v>13.6</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="I14" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="4">
+        <f>(L13/200) *100</f>
+        <v>0.35525000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="18" x14ac:dyDescent="0.4">
+      <c r="A15" s="4">
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="U11" s="1">
+      <c r="B15" s="5">
+        <v>14</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="7">
+        <v>25</v>
+      </c>
+      <c r="E15" s="8">
+        <v>15.4</v>
+      </c>
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="V11" s="1">
+      <c r="B16" s="5">
+        <v>13.6</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="4">
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
+      <c r="B17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="4">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="4">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="4">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="4">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="4">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="4">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="4">
+        <f t="shared" si="1"/>
+        <v>170</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="4">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="4">
+        <f t="shared" si="1"/>
+        <v>190</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="4">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>